<commit_message>
'add report offset range'
</commit_message>
<xml_diff>
--- a/dcd_top_offset_range_tsmc2p_meas.xlsx
+++ b/dcd_top_offset_range_tsmc2p_meas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="82">
   <si>
     <t>Process</t>
   </si>
@@ -758,11 +758,11 @@
       <c r="U2">
         <v>0</v>
       </c>
-      <c r="V2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>36</v>
+      <c r="V2">
+        <v>-6.66624</v>
+      </c>
+      <c r="W2">
+        <v>6.65638</v>
       </c>
     </row>
     <row r="3" spans="1:23">
@@ -829,11 +829,11 @@
       <c r="U3">
         <v>0</v>
       </c>
-      <c r="V3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>36</v>
+      <c r="V3">
+        <v>-7.9208</v>
+      </c>
+      <c r="W3">
+        <v>7.85949</v>
       </c>
     </row>
     <row r="4" spans="1:23">
@@ -900,11 +900,11 @@
       <c r="U4">
         <v>0</v>
       </c>
-      <c r="V4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>36</v>
+      <c r="V4">
+        <v>-6.04503</v>
+      </c>
+      <c r="W4">
+        <v>6.07789</v>
       </c>
     </row>
     <row r="5" spans="1:23">
@@ -971,11 +971,11 @@
       <c r="U5">
         <v>0</v>
       </c>
-      <c r="V5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W5" s="2" t="s">
-        <v>36</v>
+      <c r="V5">
+        <v>-7.35354</v>
+      </c>
+      <c r="W5">
+        <v>7.36635</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -1042,11 +1042,11 @@
       <c r="U6">
         <v>0</v>
       </c>
-      <c r="V6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W6" s="2" t="s">
-        <v>36</v>
+      <c r="V6">
+        <v>-5.47758</v>
+      </c>
+      <c r="W6">
+        <v>5.47207</v>
       </c>
     </row>
     <row r="7" spans="1:23">
@@ -1113,11 +1113,11 @@
       <c r="U7">
         <v>0</v>
       </c>
-      <c r="V7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W7" s="2" t="s">
-        <v>36</v>
+      <c r="V7">
+        <v>-7.53332</v>
+      </c>
+      <c r="W7">
+        <v>7.57574</v>
       </c>
     </row>
     <row r="8" spans="1:23">
@@ -1184,11 +1184,11 @@
       <c r="U8">
         <v>0</v>
       </c>
-      <c r="V8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W8" s="2" t="s">
-        <v>36</v>
+      <c r="V8">
+        <v>-5.61293</v>
+      </c>
+      <c r="W8">
+        <v>5.61112</v>
       </c>
     </row>
     <row r="9" spans="1:23">
@@ -1255,11 +1255,11 @@
       <c r="U9">
         <v>0</v>
       </c>
-      <c r="V9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W9" s="2" t="s">
-        <v>36</v>
+      <c r="V9">
+        <v>-7.40006</v>
+      </c>
+      <c r="W9">
+        <v>7.33337</v>
       </c>
     </row>
     <row r="10" spans="1:23">
@@ -1326,11 +1326,11 @@
       <c r="U10">
         <v>0</v>
       </c>
-      <c r="V10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W10" s="2" t="s">
-        <v>36</v>
+      <c r="V10">
+        <v>-5.51945</v>
+      </c>
+      <c r="W10">
+        <v>5.56523</v>
       </c>
     </row>
     <row r="11" spans="1:23" s="1" customFormat="1">
@@ -1432,11 +1432,11 @@
       <c r="U12" s="1">
         <v>0</v>
       </c>
-      <c r="V12" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="W12" s="1" t="s">
-        <v>73</v>
+      <c r="V12" s="1">
+        <v>-7.9208</v>
+      </c>
+      <c r="W12" s="1">
+        <v>5.47207</v>
       </c>
     </row>
     <row r="13" spans="1:23" s="1" customFormat="1">
@@ -1467,11 +1467,11 @@
       <c r="U13" s="1">
         <v>0</v>
       </c>
-      <c r="V13" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="W13" s="1" t="s">
-        <v>73</v>
+      <c r="V13" s="1">
+        <v>-5.47758</v>
+      </c>
+      <c r="W13" s="1">
+        <v>7.85949</v>
       </c>
     </row>
     <row r="14" spans="1:23" s="1" customFormat="1">
@@ -1522,11 +1522,11 @@
       <c r="U18" s="1">
         <v>0</v>
       </c>
-      <c r="V18" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="W18" s="1" t="s">
-        <v>73</v>
+      <c r="V18" s="1">
+        <v>-6.614328</v>
+      </c>
+      <c r="W18" s="1">
+        <v>6.613071</v>
       </c>
     </row>
     <row r="19" spans="13:23" s="1" customFormat="1">
@@ -1557,11 +1557,11 @@
       <c r="U19" s="1">
         <v>0</v>
       </c>
-      <c r="V19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="W19" s="1" t="s">
-        <v>73</v>
+      <c r="V19" s="1">
+        <v>0.915045</v>
+      </c>
+      <c r="W19" s="1">
+        <v>0.89806</v>
       </c>
     </row>
     <row r="20" spans="13:23" s="1" customFormat="1">
@@ -1592,11 +1592,11 @@
       <c r="U20" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="V20" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="W20" s="1" t="s">
-        <v>73</v>
+      <c r="V20" s="1">
+        <v>13.834285</v>
+      </c>
+      <c r="W20" s="1">
+        <v>13.580075</v>
       </c>
     </row>
     <row r="21" spans="13:23" s="1" customFormat="1"/>

</xml_diff>

<commit_message>
'update report offset range initial ver'
</commit_message>
<xml_diff>
--- a/dcd_top_offset_range_tsmc2p_meas.xlsx
+++ b/dcd_top_offset_range_tsmc2p_meas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="80">
   <si>
     <t>Process</t>
   </si>
@@ -124,9 +124,6 @@
     <t>typical</t>
   </si>
   <si>
-    <t>error</t>
-  </si>
-  <si>
     <t>tsmc2p (1)</t>
   </si>
   <si>
@@ -233,9 +230,6 @@
   </si>
   <si>
     <t>Min</t>
-  </si>
-  <si>
-    <t>n/a</t>
   </si>
   <si>
     <t>Max</t>
@@ -266,7 +260,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,26 +276,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000 "/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -316,10 +297,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -734,29 +714,29 @@
       <c r="M2" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>36</v>
+      <c r="N2">
+        <v>49.9206</v>
+      </c>
+      <c r="O2">
+        <v>2.81984</v>
+      </c>
+      <c r="P2">
+        <v>0.0838854</v>
+      </c>
+      <c r="Q2">
+        <v>-2.65316</v>
+      </c>
+      <c r="R2">
+        <v>-49.9988</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>2.7359546</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>2.7370454</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>1.561240625</v>
       </c>
       <c r="V2">
         <v>-6.66624</v>
@@ -767,34 +747,34 @@
     </row>
     <row r="3" spans="1:23">
       <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
         <v>37</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>38</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>39</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>40</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>41</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>42</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>43</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>44</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>45</v>
-      </c>
-      <c r="J3" t="s">
-        <v>46</v>
       </c>
       <c r="K3" t="s">
         <v>33</v>
@@ -803,31 +783,31 @@
         <v>34</v>
       </c>
       <c r="M3" t="s">
-        <v>47</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>36</v>
+        <v>46</v>
+      </c>
+      <c r="N3">
+        <v>64.83929999999999</v>
+      </c>
+      <c r="O3">
+        <v>3.40027</v>
+      </c>
+      <c r="P3">
+        <v>0.0461746</v>
+      </c>
+      <c r="Q3">
+        <v>-3.2573</v>
+      </c>
+      <c r="R3">
+        <v>-65.3481</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>3.3540954</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <v>3.3034746</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <v>2.034178125</v>
       </c>
       <c r="V3">
         <v>-7.9208</v>
@@ -838,34 +818,34 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" t="s">
         <v>48</v>
       </c>
-      <c r="B4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" t="s">
-        <v>49</v>
-      </c>
       <c r="J4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K4" t="s">
         <v>33</v>
@@ -874,31 +854,31 @@
         <v>34</v>
       </c>
       <c r="M4" t="s">
-        <v>47</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>36</v>
+        <v>46</v>
+      </c>
+      <c r="N4">
+        <v>50.1411</v>
+      </c>
+      <c r="O4">
+        <v>2.45331</v>
+      </c>
+      <c r="P4">
+        <v>0.128218</v>
+      </c>
+      <c r="Q4">
+        <v>-2.04108</v>
+      </c>
+      <c r="R4">
+        <v>-49.8731</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>2.325092</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>2.169298</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>1.562721875</v>
       </c>
       <c r="V4">
         <v>-6.04503</v>
@@ -909,34 +889,34 @@
     </row>
     <row r="5" spans="1:23">
       <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
         <v>50</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>51</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>52</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>53</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>54</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>55</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>56</v>
       </c>
-      <c r="H5" t="s">
-        <v>57</v>
-      </c>
       <c r="I5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" t="s">
         <v>45</v>
-      </c>
-      <c r="J5" t="s">
-        <v>46</v>
       </c>
       <c r="K5" t="s">
         <v>33</v>
@@ -945,31 +925,31 @@
         <v>34</v>
       </c>
       <c r="M5" t="s">
-        <v>58</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>36</v>
+        <v>57</v>
+      </c>
+      <c r="N5">
+        <v>60.7701</v>
+      </c>
+      <c r="O5">
+        <v>3.08059</v>
+      </c>
+      <c r="P5">
+        <v>0.195989</v>
+      </c>
+      <c r="Q5">
+        <v>-2.73745</v>
+      </c>
+      <c r="R5">
+        <v>-60.6691</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>2.884601</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <v>2.933439</v>
       </c>
       <c r="U5">
-        <v>0</v>
+        <v>1.8974875</v>
       </c>
       <c r="V5">
         <v>-7.35354</v>
@@ -980,34 +960,34 @@
     </row>
     <row r="6" spans="1:23">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
         <v>51</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>52</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>53</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>54</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>55</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>56</v>
       </c>
-      <c r="H6" t="s">
-        <v>57</v>
-      </c>
       <c r="I6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K6" t="s">
         <v>33</v>
@@ -1016,31 +996,31 @@
         <v>34</v>
       </c>
       <c r="M6" t="s">
-        <v>58</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>36</v>
+        <v>57</v>
+      </c>
+      <c r="N6">
+        <v>45.1421</v>
+      </c>
+      <c r="O6">
+        <v>2.6589</v>
+      </c>
+      <c r="P6">
+        <v>0.074771</v>
+      </c>
+      <c r="Q6">
+        <v>-2.35402</v>
+      </c>
+      <c r="R6">
+        <v>-45.1924</v>
       </c>
       <c r="S6">
-        <v>0</v>
+        <v>2.584129</v>
       </c>
       <c r="T6">
-        <v>0</v>
+        <v>2.428791</v>
       </c>
       <c r="U6">
-        <v>0</v>
+        <v>1.4114765625</v>
       </c>
       <c r="V6">
         <v>-5.47758</v>
@@ -1051,34 +1031,34 @@
     </row>
     <row r="7" spans="1:23">
       <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
         <v>60</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>61</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>62</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>63</v>
       </c>
-      <c r="E7" t="s">
-        <v>64</v>
-      </c>
       <c r="F7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" t="s">
         <v>55</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>56</v>
       </c>
-      <c r="H7" t="s">
-        <v>57</v>
-      </c>
       <c r="I7" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" t="s">
         <v>45</v>
-      </c>
-      <c r="J7" t="s">
-        <v>46</v>
       </c>
       <c r="K7" t="s">
         <v>33</v>
@@ -1087,31 +1067,31 @@
         <v>34</v>
       </c>
       <c r="M7" t="s">
-        <v>58</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>36</v>
+        <v>57</v>
+      </c>
+      <c r="N7">
+        <v>62.4981</v>
+      </c>
+      <c r="O7">
+        <v>3.0458</v>
+      </c>
+      <c r="P7">
+        <v>0.19737</v>
+      </c>
+      <c r="Q7">
+        <v>-2.65001</v>
+      </c>
+      <c r="R7">
+        <v>-62.1518</v>
       </c>
       <c r="S7">
-        <v>0</v>
+        <v>2.84843</v>
       </c>
       <c r="T7">
-        <v>0</v>
+        <v>2.84738</v>
       </c>
       <c r="U7">
-        <v>0</v>
+        <v>1.9476546875</v>
       </c>
       <c r="V7">
         <v>-7.53332</v>
@@ -1122,34 +1102,34 @@
     </row>
     <row r="8" spans="1:23">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" t="s">
         <v>61</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>62</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>63</v>
       </c>
-      <c r="E8" t="s">
-        <v>64</v>
-      </c>
       <c r="F8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" t="s">
         <v>55</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>56</v>
       </c>
-      <c r="H8" t="s">
-        <v>57</v>
-      </c>
       <c r="I8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K8" t="s">
         <v>33</v>
@@ -1158,31 +1138,31 @@
         <v>34</v>
       </c>
       <c r="M8" t="s">
-        <v>58</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>36</v>
+        <v>57</v>
+      </c>
+      <c r="N8">
+        <v>46.2899</v>
+      </c>
+      <c r="O8">
+        <v>2.31079</v>
+      </c>
+      <c r="P8">
+        <v>0.243738</v>
+      </c>
+      <c r="Q8">
+        <v>-1.82308</v>
+      </c>
+      <c r="R8">
+        <v>-46.3085</v>
       </c>
       <c r="S8">
-        <v>0</v>
+        <v>2.067052</v>
       </c>
       <c r="T8">
-        <v>0</v>
+        <v>2.066818</v>
       </c>
       <c r="U8">
-        <v>0</v>
+        <v>1.44685</v>
       </c>
       <c r="V8">
         <v>-5.61293</v>
@@ -1193,34 +1173,34 @@
     </row>
     <row r="9" spans="1:23">
       <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" t="s">
         <v>66</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>67</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>68</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>69</v>
       </c>
-      <c r="E9" t="s">
-        <v>70</v>
-      </c>
       <c r="F9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" t="s">
         <v>55</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>56</v>
       </c>
-      <c r="H9" t="s">
-        <v>57</v>
-      </c>
       <c r="I9" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" t="s">
         <v>45</v>
-      </c>
-      <c r="J9" t="s">
-        <v>46</v>
       </c>
       <c r="K9" t="s">
         <v>33</v>
@@ -1229,31 +1209,31 @@
         <v>34</v>
       </c>
       <c r="M9" t="s">
-        <v>58</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R9" s="2" t="s">
-        <v>36</v>
+        <v>57</v>
+      </c>
+      <c r="N9">
+        <v>60.4984</v>
+      </c>
+      <c r="O9">
+        <v>3.00057</v>
+      </c>
+      <c r="P9">
+        <v>0.021662</v>
+      </c>
+      <c r="Q9">
+        <v>-2.81149</v>
+      </c>
+      <c r="R9">
+        <v>-61.0526</v>
       </c>
       <c r="S9">
-        <v>0</v>
+        <v>2.978908</v>
       </c>
       <c r="T9">
-        <v>0</v>
+        <v>2.833152</v>
       </c>
       <c r="U9">
-        <v>0</v>
+        <v>1.899234375</v>
       </c>
       <c r="V9">
         <v>-7.40006</v>
@@ -1264,34 +1244,34 @@
     </row>
     <row r="10" spans="1:23">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" t="s">
         <v>67</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>68</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>69</v>
       </c>
-      <c r="E10" t="s">
-        <v>70</v>
-      </c>
       <c r="F10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" t="s">
         <v>55</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>56</v>
       </c>
-      <c r="H10" t="s">
-        <v>57</v>
-      </c>
       <c r="I10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K10" t="s">
         <v>33</v>
@@ -1300,31 +1280,31 @@
         <v>34</v>
       </c>
       <c r="M10" t="s">
-        <v>58</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R10" s="2" t="s">
-        <v>36</v>
+        <v>57</v>
+      </c>
+      <c r="N10">
+        <v>45.9112</v>
+      </c>
+      <c r="O10">
+        <v>2.24666</v>
+      </c>
+      <c r="P10">
+        <v>0.134148</v>
+      </c>
+      <c r="Q10">
+        <v>-1.98711</v>
+      </c>
+      <c r="R10">
+        <v>-45.5374</v>
       </c>
       <c r="S10">
-        <v>0</v>
+        <v>2.112512</v>
       </c>
       <c r="T10">
-        <v>0</v>
+        <v>2.121258</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <v>1.428884375</v>
       </c>
       <c r="V10">
         <v>-5.51945</v>
@@ -1406,31 +1386,31 @@
     </row>
     <row r="12" spans="1:23" s="1" customFormat="1">
       <c r="M12" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
+      </c>
+      <c r="N12" s="1">
+        <v>45.1421</v>
+      </c>
+      <c r="O12" s="1">
+        <v>2.24666</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0.021662</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>-3.2573</v>
+      </c>
+      <c r="R12" s="1">
+        <v>-65.3481</v>
       </c>
       <c r="S12" s="1">
-        <v>0</v>
+        <v>2.067052</v>
       </c>
       <c r="T12" s="1">
-        <v>0</v>
+        <v>2.066818</v>
       </c>
       <c r="U12" s="1">
-        <v>0</v>
+        <v>1.4114765625</v>
       </c>
       <c r="V12" s="1">
         <v>-7.9208</v>
@@ -1441,31 +1421,31 @@
     </row>
     <row r="13" spans="1:23" s="1" customFormat="1">
       <c r="M13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="N13" s="1">
+        <v>64.83929999999999</v>
+      </c>
+      <c r="O13" s="1">
+        <v>3.40027</v>
+      </c>
+      <c r="P13" s="1">
+        <v>0.243738</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>-1.82308</v>
+      </c>
+      <c r="R13" s="1">
+        <v>-45.1924</v>
       </c>
       <c r="S13" s="1">
-        <v>0</v>
+        <v>3.3540954</v>
       </c>
       <c r="T13" s="1">
-        <v>0</v>
+        <v>3.3034746</v>
       </c>
       <c r="U13" s="1">
-        <v>0</v>
+        <v>2.034178125</v>
       </c>
       <c r="V13" s="1">
         <v>-5.47758</v>
@@ -1476,51 +1456,51 @@
     </row>
     <row r="14" spans="1:23" s="1" customFormat="1">
       <c r="M14" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:23" s="1" customFormat="1">
       <c r="M15" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:23" s="1" customFormat="1">
       <c r="M16" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="13:23" s="1" customFormat="1">
       <c r="M17" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="13:23" s="1" customFormat="1">
       <c r="M18" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="R18" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
+      </c>
+      <c r="N18" s="1">
+        <v>54.0012</v>
+      </c>
+      <c r="O18" s="1">
+        <v>2.779637</v>
+      </c>
+      <c r="P18" s="1">
+        <v>0.1251062</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>-2.479411</v>
+      </c>
+      <c r="R18" s="1">
+        <v>-54.01464</v>
       </c>
       <c r="S18" s="1">
-        <v>0</v>
+        <v>2.65453</v>
       </c>
       <c r="T18" s="1">
-        <v>0</v>
+        <v>2.604517</v>
       </c>
       <c r="U18" s="1">
-        <v>0</v>
+        <v>1.687748</v>
       </c>
       <c r="V18" s="1">
         <v>-6.614328</v>
@@ -1531,31 +1511,31 @@
     </row>
     <row r="19" spans="13:23" s="1" customFormat="1">
       <c r="M19" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="R19" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
+      </c>
+      <c r="N19" s="1">
+        <v>7.547192</v>
+      </c>
+      <c r="O19" s="1">
+        <v>0.368477</v>
+      </c>
+      <c r="P19" s="1">
+        <v>0.071161</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>0.437449</v>
+      </c>
+      <c r="R19" s="1">
+        <v>7.679951</v>
       </c>
       <c r="S19" s="1">
-        <v>0</v>
+        <v>0.400579</v>
       </c>
       <c r="T19" s="1">
-        <v>0</v>
+        <v>0.40394</v>
       </c>
       <c r="U19" s="1">
-        <v>0</v>
+        <v>0.237881</v>
       </c>
       <c r="V19" s="1">
         <v>0.915045</v>
@@ -1566,31 +1546,31 @@
     </row>
     <row r="20" spans="13:23" s="1" customFormat="1">
       <c r="M20" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="S20" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="T20" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="U20" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
+      </c>
+      <c r="N20" s="1">
+        <v>13.975971</v>
+      </c>
+      <c r="O20" s="1">
+        <v>13.256299</v>
+      </c>
+      <c r="P20" s="1">
+        <v>56.880474</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>17.643263</v>
+      </c>
+      <c r="R20" s="1">
+        <v>14.218277</v>
+      </c>
+      <c r="S20" s="1">
+        <v>15.090393</v>
+      </c>
+      <c r="T20" s="1">
+        <v>15.50921</v>
+      </c>
+      <c r="U20" s="1">
+        <v>14.09458</v>
       </c>
       <c r="V20" s="1">
         <v>13.834285</v>

</xml_diff>